<commit_message>
speed ups to runtime system
</commit_message>
<xml_diff>
--- a/wip/timming/benchmarks.xlsx
+++ b/wip/timming/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="269"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="269" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fannkuch-redux" sheetId="1" r:id="rId1"/>
@@ -245,7 +245,7 @@
                   <c:v>96.064999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>57.243333333333339</c:v>
+                  <c:v>53.200333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9.838000000000001</c:v>
@@ -273,11 +273,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="49321984"/>
-        <c:axId val="118308864"/>
+        <c:axId val="110497280"/>
+        <c:axId val="70358080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49321984"/>
+        <c:axId val="110497280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -287,7 +287,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118308864"/>
+        <c:crossAx val="70358080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -296,7 +296,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118308864"/>
+        <c:axId val="70358080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -313,7 +313,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49321984"/>
+        <c:crossAx val="110497280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -508,11 +508,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="102509568"/>
-        <c:axId val="88412096"/>
+        <c:axId val="111645184"/>
+        <c:axId val="70359808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102509568"/>
+        <c:axId val="111645184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -521,7 +521,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88412096"/>
+        <c:crossAx val="70359808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -529,7 +529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88412096"/>
+        <c:axId val="70359808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +546,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="102509568"/>
+        <c:crossAx val="111645184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -955,7 +955,7 @@
         <v>3820.2640000000001</v>
       </c>
       <c r="E2" s="1">
-        <f>AVERAGE(B2:D2)</f>
+        <f t="shared" ref="E2:E11" si="0">AVERAGE(B2:D2)</f>
         <v>3820.2640000000006</v>
       </c>
     </row>
@@ -976,7 +976,7 @@
         <v>2285.4789999999998</v>
       </c>
       <c r="E3" s="1">
-        <f>AVERAGE(B3:D3)</f>
+        <f t="shared" si="0"/>
         <v>2285.4789999999998</v>
       </c>
     </row>
@@ -997,7 +997,7 @@
         <v>1745.5170000000001</v>
       </c>
       <c r="E4" s="1">
-        <f>AVERAGE(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>1745.1403333333335</v>
       </c>
     </row>
@@ -1018,7 +1018,7 @@
         <v>1541.0440000000001</v>
       </c>
       <c r="E5" s="1">
-        <f>AVERAGE(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>1544.0173333333332</v>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
         <v>423.87</v>
       </c>
       <c r="E6" s="1">
-        <f>AVERAGE(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>422.70633333333336</v>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
         <v>172.91800000000001</v>
       </c>
       <c r="E7" s="1">
-        <f>AVERAGE(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>172.97666666666669</v>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
         <v>163.55199999999999</v>
       </c>
       <c r="E8" s="1">
-        <f>AVERAGE(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>155.02233333333334</v>
       </c>
     </row>
@@ -1102,7 +1102,7 @@
         <v>58.334000000000003</v>
       </c>
       <c r="E9" s="1">
-        <f>AVERAGE(B9:D9)</f>
+        <f t="shared" si="0"/>
         <v>58.334000000000003</v>
       </c>
     </row>
@@ -1123,7 +1123,7 @@
         <v>49.734999999999999</v>
       </c>
       <c r="E10" s="1">
-        <f>AVERAGE(B10:D10)</f>
+        <f t="shared" si="0"/>
         <v>49.846333333333327</v>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
         <v>46.744</v>
       </c>
       <c r="E11" s="1">
-        <f>AVERAGE(B11:D11)</f>
+        <f t="shared" si="0"/>
         <v>47.474666666666671</v>
       </c>
     </row>
@@ -1245,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1257,8 +1257,8 @@
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1275,11 +1275,11 @@
         <v>230.72300000000001</v>
       </c>
       <c r="E2" s="1">
-        <f>AVERAGE(B2:D2)</f>
+        <f t="shared" ref="E2:E11" si="0">AVERAGE(B2:D2)</f>
         <v>230.57600000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1296,11 +1296,27 @@
         <v>212.679</v>
       </c>
       <c r="E3" s="1">
-        <f>AVERAGE(B3:D3)</f>
+        <f t="shared" si="0"/>
         <v>208.63366666666664</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <f>SUM(0*60+53.251)</f>
+        <v>53.250999999999998</v>
+      </c>
+      <c r="H3">
+        <f>SUM(0*60+53.068)</f>
+        <v>53.067999999999998</v>
+      </c>
+      <c r="I3">
+        <f>SUM(0*60+53.282)</f>
+        <v>53.281999999999996</v>
+      </c>
+      <c r="J3">
+        <f>AVERAGE(G3:I3)</f>
+        <v>53.200333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1317,11 +1333,15 @@
         <v>158.816</v>
       </c>
       <c r="E4" s="1">
-        <f>AVERAGE(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>157.83133333333333</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <f>1-J3/E7</f>
+        <v>7.062831188493579E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1338,11 +1358,11 @@
         <v>157.02000000000001</v>
       </c>
       <c r="E5" s="1">
-        <f>AVERAGE(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>157.45599999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1359,11 +1379,11 @@
         <v>96.497</v>
       </c>
       <c r="E6" s="1">
-        <f>AVERAGE(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>96.064999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1380,11 +1400,11 @@
         <v>58.031999999999996</v>
       </c>
       <c r="E7" s="1">
-        <f>AVERAGE(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>57.243333333333339</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1401,11 +1421,11 @@
         <v>9.5660000000000007</v>
       </c>
       <c r="E8" s="1">
-        <f>AVERAGE(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>9.838000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1422,11 +1442,11 @@
         <v>7.4009999999999998</v>
       </c>
       <c r="E9" s="1">
-        <f>AVERAGE(B9:D9)</f>
+        <f t="shared" si="0"/>
         <v>8.1603333333333321</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1443,11 +1463,11 @@
         <v>7.8949999999999996</v>
       </c>
       <c r="E10" s="1">
-        <f>AVERAGE(B10:D10)</f>
+        <f t="shared" si="0"/>
         <v>7.9379999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1484,7 @@
         <v>4.0380000000000003</v>
       </c>
       <c r="E11" s="1">
-        <f>AVERAGE(B11:D11)</f>
+        <f t="shared" si="0"/>
         <v>4.0179999999999998</v>
       </c>
     </row>
@@ -1513,7 +1533,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="2">
-        <v>57.243333333333339</v>
+        <v>53.200333333333333</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updating code for windows
</commit_message>
<xml_diff>
--- a/wip/timming/benchmarks.xlsx
+++ b/wip/timming/benchmarks.xlsx
@@ -175,6 +175,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Time (secs)</c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -273,11 +276,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="110235136"/>
-        <c:axId val="66950208"/>
+        <c:axId val="97746432"/>
+        <c:axId val="77960256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110235136"/>
+        <c:axId val="97746432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -287,7 +290,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66950208"/>
+        <c:crossAx val="77960256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -296,7 +299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66950208"/>
+        <c:axId val="77960256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -313,7 +316,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="110235136"/>
+        <c:crossAx val="97746432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -410,6 +413,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Time (secs)</c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -508,11 +514,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="113746432"/>
-        <c:axId val="66951936"/>
+        <c:axId val="109355520"/>
+        <c:axId val="77961984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113746432"/>
+        <c:axId val="109355520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -521,7 +527,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66951936"/>
+        <c:crossAx val="77961984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -529,7 +535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66951936"/>
+        <c:axId val="77961984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +552,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="113746432"/>
+        <c:crossAx val="109355520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1253,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
merge from the experimental branch
</commit_message>
<xml_diff>
--- a/wip/timming/benchmarks.xlsx
+++ b/wip/timming/benchmarks.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" tabRatio="353" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" tabRatio="353" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="fannkuch-redux" sheetId="1" r:id="rId1"/>
     <sheet name="fasta" sheetId="2" r:id="rId2"/>
     <sheet name="mandelbrot" sheetId="3" r:id="rId3"/>
-    <sheet name="nroot" sheetId="4" r:id="rId4"/>
+    <sheet name="spectralnorm" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'fannkuch-redux'!$A$1:$E$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fasta!$A$1:$E$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">mandelbrot!$E$1:$E$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">nroot!$E$1:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">spectralnorm!$E$1:$E$11</definedName>
   </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
@@ -296,11 +297,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="114961920"/>
-        <c:axId val="78026368"/>
+        <c:axId val="108346880"/>
+        <c:axId val="95524480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114961920"/>
+        <c:axId val="108346880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -310,7 +311,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78026368"/>
+        <c:crossAx val="95524480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -319,7 +320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78026368"/>
+        <c:axId val="95524480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -336,7 +337,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="114961920"/>
+        <c:crossAx val="108346880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -420,6 +421,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -533,11 +535,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115589632"/>
-        <c:axId val="78028096"/>
+        <c:axId val="109498880"/>
+        <c:axId val="95526208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115589632"/>
+        <c:axId val="109498880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +548,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78028096"/>
+        <c:crossAx val="95526208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -554,7 +556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78028096"/>
+        <c:axId val="95526208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -571,13 +573,14 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="115589632"/>
+        <c:crossAx val="109498880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -764,11 +767,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115591168"/>
-        <c:axId val="115344512"/>
+        <c:axId val="109500416"/>
+        <c:axId val="42796160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115591168"/>
+        <c:axId val="109500416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -778,7 +781,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115344512"/>
+        <c:crossAx val="42796160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -787,7 +790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115344512"/>
+        <c:axId val="42796160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,7 +807,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="115591168"/>
+        <c:crossAx val="109500416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -867,19 +870,7 @@
               <a:rPr lang="en-US" b="1" i="0" u="none" strike="noStrike">
                 <a:effectLst/>
               </a:rPr>
-              <a:t> CLBG:</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" i="0" u="none" strike="noStrike">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>n-body n=50000000</a:t>
+              <a:t> CLBG spectral-norm n=5500</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -909,20 +900,20 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>nroot!$A$2:$A$11</c:f>
+              <c:f>spectralnorm!$A$2:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Haskell GHC (7.1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Perl (5.14)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>JRuby (1.5)</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Ruby (1.9.2)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Perl (5.14)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>JRuby (1.5)</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Python (3.2)</c:v>
@@ -937,49 +928,49 @@
                   <c:v>Ocaml (3.12)</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Java (server 1.7.0)</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>C (4.6)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Java (server 1.7.0)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>nroot!$E$2:$E$11</c:f>
+              <c:f>spectralnorm!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1884.7125000000001</c:v>
+                  <c:v>3678.3850000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1337.83</c:v>
+                  <c:v>828.01899999999989</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1302.5520000000001</c:v>
+                  <c:v>492.52766666666668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>925.50700000000006</c:v>
+                  <c:v>487.02600000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>837.95749999999998</c:v>
+                  <c:v>366.01366666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>632.41733333333332</c:v>
+                  <c:v>17.100999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89.442000000000007</c:v>
+                  <c:v>11.729333333333335</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.437666666666669</c:v>
+                  <c:v>9.59</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.238999999999999</c:v>
+                  <c:v>5.3659999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.2043333333333326</c:v>
+                  <c:v>3.1173333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -995,11 +986,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="49372672"/>
-        <c:axId val="43091072"/>
+        <c:axId val="144259072"/>
+        <c:axId val="96918848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49372672"/>
+        <c:axId val="144259072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,7 +1000,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43091072"/>
+        <c:crossAx val="96918848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1018,7 +1009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43091072"/>
+        <c:axId val="96918848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,7 +1026,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49372672"/>
+        <c:crossAx val="144259072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1165,20 +1156,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>195264</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>157164</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>176214</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>100014</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2137,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2367,7 +2358,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2381,67 +2372,79 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <f>SUM(31*60+23.621)</f>
-        <v>1883.6210000000001</v>
+        <f>SUM(61*60+52.547)</f>
+        <v>3712.547</v>
       </c>
       <c r="C2">
-        <f>SUM(31*60+25.804)</f>
-        <v>1885.8040000000001</v>
+        <f>SUM(60*60+44.223)</f>
+        <v>3644.223</v>
       </c>
       <c r="E2" s="3">
         <f>AVERAGE(B2:D2)</f>
-        <v>1884.7125000000001</v>
+        <v>3678.3850000000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <f>SUM(22*60+23.863)</f>
-        <v>1343.8630000000001</v>
+        <f>SUM(13*60+34.31)</f>
+        <v>814.31</v>
       </c>
       <c r="C3">
-        <f>SUM(22*60+11.797)</f>
-        <v>1331.797</v>
+        <f>SUM(14*60+0.576)</f>
+        <v>840.57600000000002</v>
+      </c>
+      <c r="D3">
+        <f>SUM(13*60+49.171)</f>
+        <v>829.17100000000005</v>
       </c>
       <c r="E3" s="3">
         <f>AVERAGE(B3:D3)</f>
-        <v>1337.83</v>
+        <v>828.01899999999989</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <f>SUM(21*60+39.259)</f>
-        <v>1299.259</v>
+        <f>SUM(8*60+2.875)</f>
+        <v>482.875</v>
       </c>
       <c r="C4">
-        <f>SUM(21*60+45.845)</f>
-        <v>1305.845</v>
+        <f>SUM(8*60+17.876)</f>
+        <v>497.87599999999998</v>
+      </c>
+      <c r="D4">
+        <f>SUM(8*60+16.832)</f>
+        <v>496.83199999999999</v>
       </c>
       <c r="E4" s="3">
         <f>AVERAGE(B4:D4)</f>
-        <v>1302.5520000000001</v>
+        <v>492.52766666666668</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <f>SUM(15*60+13.488)</f>
-        <v>913.48800000000006</v>
+        <f>SUM(8*60+6.412)</f>
+        <v>486.41199999999998</v>
       </c>
       <c r="C5">
-        <f>SUM(15*60+37.526)</f>
-        <v>937.52599999999995</v>
+        <f>SUM(8*60+6.079)</f>
+        <v>486.07900000000001</v>
+      </c>
+      <c r="D5">
+        <f>SUM(8*60+8.587)</f>
+        <v>488.58699999999999</v>
       </c>
       <c r="E5" s="3">
         <f>AVERAGE(B5:D5)</f>
-        <v>925.50700000000006</v>
+        <v>487.02600000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2449,16 +2452,20 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <f>SUM(14*60+10.809)</f>
-        <v>850.80899999999997</v>
+        <f>SUM(6*60+5.222)</f>
+        <v>365.22199999999998</v>
       </c>
       <c r="C6">
-        <f>SUM(13*60+45.106)</f>
-        <v>825.10599999999999</v>
+        <f>SUM(6*60+3.848)</f>
+        <v>363.84800000000001</v>
+      </c>
+      <c r="D6">
+        <f>SUM(6*60+8.971)</f>
+        <v>368.971</v>
       </c>
       <c r="E6" s="3">
         <f>AVERAGE(B6:D6)</f>
-        <v>837.95749999999998</v>
+        <v>366.01366666666667</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2466,20 +2473,20 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <f>SUM(10*60+29.511)</f>
-        <v>629.51099999999997</v>
+        <f>SUM(0*60+17.128)</f>
+        <v>17.128</v>
       </c>
       <c r="C7">
-        <f>SUM(10*60+37.887)</f>
-        <v>637.88699999999994</v>
+        <f>SUM(0*60+17.142)</f>
+        <v>17.141999999999999</v>
       </c>
       <c r="D7">
-        <f>SUM(10*60+29.854)</f>
-        <v>629.85400000000004</v>
+        <f>SUM(0*60+17.033)</f>
+        <v>17.033000000000001</v>
       </c>
       <c r="E7" s="3">
         <f>AVERAGE(B7:D7)</f>
-        <v>632.41733333333332</v>
+        <v>17.100999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2487,20 +2494,20 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <f>SUM(1*60+29.343)</f>
-        <v>89.343000000000004</v>
+        <f>SUM(0*60+11.709)</f>
+        <v>11.709</v>
       </c>
       <c r="C8">
-        <f>SUM(1*60+29.214)</f>
-        <v>89.213999999999999</v>
+        <f>SUM(0*60+11.854)</f>
+        <v>11.853999999999999</v>
       </c>
       <c r="D8">
-        <f>SUM(1*60+29.769)</f>
-        <v>89.769000000000005</v>
+        <f>SUM(0*60+11.625)</f>
+        <v>11.625</v>
       </c>
       <c r="E8" s="3">
         <f>AVERAGE(B8:D8)</f>
-        <v>89.442000000000007</v>
+        <v>11.729333333333335</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2508,62 +2515,62 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <f>SUM(0*60+20.397)</f>
-        <v>20.396999999999998</v>
+        <f>SUM(0*60+9.609)</f>
+        <v>9.609</v>
       </c>
       <c r="C9">
-        <f>SUM(0*60+20.396)</f>
-        <v>20.396000000000001</v>
+        <f>SUM(0*60+9.586)</f>
+        <v>9.5860000000000003</v>
       </c>
       <c r="D9">
-        <f>SUM(0*60+20.52)</f>
-        <v>20.52</v>
+        <f>SUM(0*60+9.575)</f>
+        <v>9.5749999999999993</v>
       </c>
       <c r="E9" s="3">
         <f>AVERAGE(B9:D9)</f>
-        <v>20.437666666666669</v>
+        <v>9.59</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <f>SUM(0*60+9.26)</f>
-        <v>9.26</v>
+        <f>SUM(0*60+5.596)</f>
+        <v>5.5960000000000001</v>
       </c>
       <c r="C10">
-        <f>SUM(0*60+9.324)</f>
-        <v>9.3239999999999998</v>
+        <f>SUM(0*60+5.244)</f>
+        <v>5.2439999999999998</v>
       </c>
       <c r="D10">
-        <f>SUM(0*60+9.133)</f>
-        <v>9.1329999999999991</v>
+        <f>SUM(0*60+5.258)</f>
+        <v>5.258</v>
       </c>
       <c r="E10" s="3">
         <f>AVERAGE(B10:D10)</f>
-        <v>9.238999999999999</v>
+        <v>5.3659999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <f>SUM(0*60+9.214)</f>
-        <v>9.2140000000000004</v>
+        <f>SUM(0*60+3.103)</f>
+        <v>3.1030000000000002</v>
       </c>
       <c r="C11">
-        <f>SUM(0*60+9.15)</f>
-        <v>9.15</v>
+        <f>SUM(0*60+3.138)</f>
+        <v>3.1379999999999999</v>
       </c>
       <c r="D11">
-        <f>SUM(0*60+9.249)</f>
-        <v>9.2490000000000006</v>
+        <f>SUM(0*60+3.111)</f>
+        <v>3.1110000000000002</v>
       </c>
       <c r="E11" s="3">
         <f>AVERAGE(B11:D11)</f>
-        <v>9.2043333333333326</v>
+        <v>3.1173333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -2573,6 +2580,24 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="A1:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>